<commit_message>
"mise à jours des absences 03/11/2016
</commit_message>
<xml_diff>
--- a/absences_travail_tp.xlsx
+++ b/absences_travail_tp.xlsx
@@ -32,7 +32,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="I4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicateur sur 100</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G47" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicateur sur 100</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I47" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,12 +85,26 @@
         </r>
       </text>
     </comment>
+    <comment ref="I87" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Indicateur sur 100
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="324">
   <si>
     <t>N°Ins</t>
   </si>
@@ -1024,6 +1064,18 @@
   </si>
   <si>
     <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <t>KADADA</t>
+  </si>
+  <si>
+    <t>SALAH EDDINE</t>
+  </si>
+  <si>
+    <t>A(malade ?)</t>
+  </si>
+  <si>
+    <t>(Sorti avant le TP ?)</t>
   </si>
 </sst>
 </file>
@@ -1253,7 +1305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1364,6 +1416,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1666,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1681,9 +1736,11 @@
     <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" style="20" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="39" t="s">
         <v>36</v>
       </c>
@@ -1691,7 +1748,7 @@
       <c r="C1" s="39"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="38" t="s">
         <v>37</v>
       </c>
@@ -1699,8 +1756,9 @@
       <c r="C2" s="38"/>
       <c r="D2" s="8"/>
       <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1708,8 +1766,12 @@
         <v>42670</v>
       </c>
       <c r="G3" s="37"/>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="37">
+        <v>42677</v>
+      </c>
+      <c r="I3" s="37"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="29"/>
       <c r="B4" s="30" t="s">
         <v>0</v>
@@ -1729,8 +1791,14 @@
       <c r="G4" s="33" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="I4" s="33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -1750,8 +1818,12 @@
       <c r="G5" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="24"/>
+      <c r="I5" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -1771,8 +1843,12 @@
       <c r="G6" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="24"/>
+      <c r="I6" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -1792,8 +1868,12 @@
       <c r="G7" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="24"/>
+      <c r="I7" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -1813,8 +1893,12 @@
       <c r="G8" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="H8" s="24"/>
+      <c r="I8" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -1834,8 +1918,12 @@
       <c r="G9" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="H9" s="24"/>
+      <c r="I9" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1855,8 +1943,12 @@
         <v>315</v>
       </c>
       <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="24"/>
+      <c r="I10" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -1876,8 +1968,12 @@
       <c r="G11" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="24"/>
+      <c r="I11" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1897,8 +1993,12 @@
       <c r="G12" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="H12" s="24"/>
+      <c r="I12" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1918,8 +2018,12 @@
       <c r="G13" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="H13" s="24"/>
+      <c r="I13" s="25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1939,8 +2043,12 @@
         <v>315</v>
       </c>
       <c r="G14" s="25"/>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="H14" s="24"/>
+      <c r="I14" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1960,8 +2068,12 @@
       <c r="G15" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="H15" s="24"/>
+      <c r="I15" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1981,8 +2093,12 @@
       <c r="G16" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="H16" s="24"/>
+      <c r="I16" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -2002,8 +2118,12 @@
         <v>315</v>
       </c>
       <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="H17" s="24"/>
+      <c r="I17" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -2023,8 +2143,12 @@
         <v>315</v>
       </c>
       <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="H18" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I18" s="25"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -2044,8 +2168,12 @@
         <v>315</v>
       </c>
       <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="H19" s="26"/>
+      <c r="I19" s="25" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -2065,8 +2193,12 @@
       <c r="G20" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="H20" s="24"/>
+      <c r="I20" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -2086,8 +2218,12 @@
       <c r="G21" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="H21" s="24"/>
+      <c r="I21" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -2107,8 +2243,12 @@
         <v>315</v>
       </c>
       <c r="G22" s="25"/>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="H22" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I22" s="25"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="3">
         <v>19</v>
       </c>
@@ -2128,8 +2268,12 @@
       <c r="G23" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="H23" s="24"/>
+      <c r="I23" s="25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="3">
         <v>20</v>
       </c>
@@ -2149,8 +2293,12 @@
         <v>315</v>
       </c>
       <c r="G24" s="25"/>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="H24" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I24" s="25"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="3">
         <v>21</v>
       </c>
@@ -2167,9 +2315,15 @@
         <v>1</v>
       </c>
       <c r="F25" s="24"/>
-      <c r="G25" s="25"/>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="G25" s="25">
+        <v>70</v>
+      </c>
+      <c r="H25" s="40"/>
+      <c r="I25" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="3">
         <v>22</v>
       </c>
@@ -2189,8 +2343,12 @@
         <v>315</v>
       </c>
       <c r="G26" s="25"/>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="H26" s="24"/>
+      <c r="I26" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="3">
         <v>23</v>
       </c>
@@ -2210,8 +2368,12 @@
       <c r="G27" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="24"/>
+      <c r="I27" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="3">
         <v>24</v>
       </c>
@@ -2231,8 +2393,12 @@
         <v>315</v>
       </c>
       <c r="G28" s="25"/>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="H28" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I28" s="25"/>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" s="3">
         <v>25</v>
       </c>
@@ -2252,8 +2418,12 @@
         <v>315</v>
       </c>
       <c r="G29" s="25"/>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="24"/>
+      <c r="I29" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" s="3">
         <v>26</v>
       </c>
@@ -2273,8 +2443,12 @@
       <c r="G30" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="24"/>
+      <c r="I30" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" s="3">
         <v>27</v>
       </c>
@@ -2294,8 +2468,12 @@
         <v>315</v>
       </c>
       <c r="G31" s="25"/>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" s="3">
         <v>28</v>
       </c>
@@ -2315,8 +2493,12 @@
       <c r="G32" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="24"/>
+      <c r="I32" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" s="3">
         <v>29</v>
       </c>
@@ -2336,8 +2518,12 @@
       <c r="G33" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="24"/>
+      <c r="I33" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" s="3">
         <v>30</v>
       </c>
@@ -2357,8 +2543,12 @@
       <c r="G34" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="24"/>
+      <c r="I34" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" s="3">
         <v>31</v>
       </c>
@@ -2378,8 +2568,12 @@
         <v>315</v>
       </c>
       <c r="G35" s="25"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="24"/>
+      <c r="I35" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" s="3">
         <v>32</v>
       </c>
@@ -2399,8 +2593,12 @@
       <c r="G36" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="24"/>
+      <c r="I36" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" s="3">
         <v>33</v>
       </c>
@@ -2420,8 +2618,12 @@
       <c r="G37" s="27">
         <v>90</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="24"/>
+      <c r="I37" s="27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" s="3">
         <v>34</v>
       </c>
@@ -2441,8 +2643,12 @@
       <c r="G38" s="27">
         <v>70</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="24"/>
+      <c r="I38" s="27">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" s="3">
         <v>35</v>
       </c>
@@ -2462,8 +2668,12 @@
       <c r="G39" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="24"/>
+      <c r="I39" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" s="19">
         <v>36</v>
       </c>
@@ -2483,8 +2693,14 @@
       <c r="G40" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I40" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" s="3">
         <v>37</v>
       </c>
@@ -2504,17 +2720,29 @@
       <c r="G41" s="36">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I41" s="36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" s="5"/>
       <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
+      <c r="C42" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="D42" s="16" t="s">
+        <v>321</v>
+      </c>
       <c r="E42" s="4"/>
       <c r="F42" s="5"/>
       <c r="G42" s="21"/>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" s="5"/>
+      <c r="I42" s="21"/>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" s="5"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
@@ -2522,8 +2750,10 @@
       <c r="E43" s="4"/>
       <c r="F43" s="5"/>
       <c r="G43" s="21"/>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" s="5"/>
+      <c r="I43" s="21"/>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44" s="39" t="s">
         <v>36</v>
       </c>
@@ -2533,8 +2763,10 @@
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="21"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="H44" s="5"/>
+      <c r="I44" s="21"/>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="38" t="s">
         <v>135</v>
       </c>
@@ -2544,8 +2776,10 @@
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="21"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" s="5"/>
+      <c r="I45" s="21"/>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46" s="12"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -2555,8 +2789,12 @@
         <v>42670</v>
       </c>
       <c r="G46" s="37"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" s="37">
+        <v>42677</v>
+      </c>
+      <c r="I46" s="37"/>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47" s="29"/>
       <c r="B47" s="30" t="s">
         <v>0</v>
@@ -2576,8 +2814,14 @@
       <c r="G47" s="33" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="I47" s="33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48" s="6">
         <v>1</v>
       </c>
@@ -2597,8 +2841,12 @@
         <v>315</v>
       </c>
       <c r="G48" s="25"/>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I48" s="25"/>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="3">
         <v>2</v>
       </c>
@@ -2618,8 +2866,12 @@
         <v>315</v>
       </c>
       <c r="G49" s="25"/>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" s="26"/>
+      <c r="I49" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50" s="6">
         <v>3</v>
       </c>
@@ -2639,8 +2891,12 @@
       <c r="G50" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" s="26"/>
+      <c r="I50" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="3">
         <v>4</v>
       </c>
@@ -2660,8 +2916,12 @@
       <c r="G51" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" s="26"/>
+      <c r="I51" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="6">
         <v>5</v>
       </c>
@@ -2681,8 +2941,12 @@
       <c r="G52" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" s="26"/>
+      <c r="I52" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53" s="3">
         <v>6</v>
       </c>
@@ -2702,8 +2966,12 @@
       <c r="G53" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="26"/>
+      <c r="I53" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54" s="6">
         <v>7</v>
       </c>
@@ -2723,8 +2991,12 @@
       <c r="G54" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" s="26"/>
+      <c r="I54" s="25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55" s="3">
         <v>8</v>
       </c>
@@ -2744,8 +3016,12 @@
         <v>315</v>
       </c>
       <c r="G55" s="25"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I55" s="25"/>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56" s="6">
         <v>9</v>
       </c>
@@ -2762,9 +3038,15 @@
         <v>2</v>
       </c>
       <c r="F56" s="24"/>
-      <c r="G56" s="25"/>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="G56" s="25">
+        <v>50</v>
+      </c>
+      <c r="H56" s="26"/>
+      <c r="I56" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57" s="3">
         <v>10</v>
       </c>
@@ -2784,8 +3066,12 @@
         <v>315</v>
       </c>
       <c r="G57" s="25"/>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I57" s="25"/>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58" s="6">
         <v>11</v>
       </c>
@@ -2805,8 +3091,12 @@
         <v>315</v>
       </c>
       <c r="G58" s="25"/>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I58" s="25"/>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59" s="3">
         <v>12</v>
       </c>
@@ -2826,8 +3116,12 @@
       <c r="G59" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" s="26"/>
+      <c r="I59" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="6">
         <v>13</v>
       </c>
@@ -2847,8 +3141,12 @@
       <c r="G60" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" s="26"/>
+      <c r="I60" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61" s="3">
         <v>14</v>
       </c>
@@ -2868,8 +3166,12 @@
       <c r="G61" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" s="26"/>
+      <c r="I61" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62" s="6">
         <v>15</v>
       </c>
@@ -2889,8 +3191,12 @@
       <c r="G62" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" s="26"/>
+      <c r="I62" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63" s="3">
         <v>16</v>
       </c>
@@ -2910,8 +3216,12 @@
       <c r="G63" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" s="26"/>
+      <c r="I63" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64" s="6">
         <v>17</v>
       </c>
@@ -2931,8 +3241,12 @@
       <c r="G64" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="H64" s="26"/>
+      <c r="I64" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" s="3">
         <v>18</v>
       </c>
@@ -2952,8 +3266,12 @@
       <c r="G65" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="H65" s="26"/>
+      <c r="I65" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" s="6">
         <v>19</v>
       </c>
@@ -2973,8 +3291,12 @@
       <c r="G66" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="H66" s="26"/>
+      <c r="I66" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" s="3">
         <v>20</v>
       </c>
@@ -2994,8 +3316,12 @@
       <c r="G67" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="H67" s="26"/>
+      <c r="I67" s="25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68" s="6">
         <v>21</v>
       </c>
@@ -3015,8 +3341,12 @@
         <v>315</v>
       </c>
       <c r="G68" s="25"/>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="H68" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I68" s="25"/>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69" s="3">
         <v>22</v>
       </c>
@@ -3036,8 +3366,12 @@
       <c r="G69" s="27">
         <v>80</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="H69" s="26"/>
+      <c r="I69" s="27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70" s="6">
         <v>23</v>
       </c>
@@ -3057,8 +3391,12 @@
         <v>315</v>
       </c>
       <c r="G70" s="25"/>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="H70" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I70" s="25"/>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71" s="3">
         <v>24</v>
       </c>
@@ -3078,8 +3416,12 @@
         <v>315</v>
       </c>
       <c r="G71" s="25"/>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="H71" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I71" s="25"/>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72" s="6">
         <v>25</v>
       </c>
@@ -3099,8 +3441,12 @@
         <v>315</v>
       </c>
       <c r="G72" s="25"/>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="H72" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I72" s="25"/>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="3">
         <v>26</v>
       </c>
@@ -3120,8 +3466,12 @@
         <v>315</v>
       </c>
       <c r="G73" s="25"/>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="H73" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I73" s="25"/>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" s="6">
         <v>27</v>
       </c>
@@ -3141,8 +3491,12 @@
       <c r="G74" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="H74" s="26"/>
+      <c r="I74" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" s="3">
         <v>28</v>
       </c>
@@ -3162,8 +3516,12 @@
       <c r="G75" s="27">
         <v>70</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="H75" s="26"/>
+      <c r="I75" s="27">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" s="3">
         <v>29</v>
       </c>
@@ -3183,8 +3541,12 @@
         <v>315</v>
       </c>
       <c r="G76" s="25"/>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="H76" s="26"/>
+      <c r="I76" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" s="6">
         <v>30</v>
       </c>
@@ -3204,8 +3566,12 @@
       <c r="G77" s="27">
         <v>90</v>
       </c>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="H77" s="26"/>
+      <c r="I77" s="27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" s="3">
         <v>31</v>
       </c>
@@ -3225,8 +3591,12 @@
       <c r="G78" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="H78" s="26"/>
+      <c r="I78" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" s="3">
         <v>32</v>
       </c>
@@ -3246,8 +3616,12 @@
       <c r="G79" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="H79" s="26"/>
+      <c r="I79" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80" s="6">
         <v>33</v>
       </c>
@@ -3267,8 +3641,12 @@
         <v>315</v>
       </c>
       <c r="G80" s="25"/>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="H80" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I80" s="25"/>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81" s="3">
         <v>34</v>
       </c>
@@ -3288,8 +3666,12 @@
         <v>315</v>
       </c>
       <c r="G81" s="25"/>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81" s="26"/>
+      <c r="I81" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82" s="6">
         <v>35</v>
       </c>
@@ -3309,8 +3691,12 @@
         <v>315</v>
       </c>
       <c r="G82" s="25"/>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I82" s="25"/>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83" s="3">
         <v>36</v>
       </c>
@@ -3330,8 +3716,12 @@
         <v>315</v>
       </c>
       <c r="G83" s="25"/>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I83" s="25"/>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84" s="5"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -3339,8 +3729,10 @@
       <c r="E84" s="17"/>
       <c r="F84" s="5"/>
       <c r="G84" s="21"/>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="H84" s="5"/>
+      <c r="I84" s="21"/>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85" s="15"/>
       <c r="B85" s="9" t="s">
         <v>36</v>
@@ -3350,8 +3742,10 @@
       <c r="E85" s="15"/>
       <c r="F85" s="34"/>
       <c r="G85" s="35"/>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="H85" s="34"/>
+      <c r="I85" s="35"/>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86" s="15"/>
       <c r="B86" s="10" t="s">
         <v>223</v>
@@ -3363,8 +3757,12 @@
         <v>42670</v>
       </c>
       <c r="G86" s="37"/>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="H86" s="37">
+        <v>42677</v>
+      </c>
+      <c r="I86" s="37"/>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87" s="29"/>
       <c r="B87" s="30" t="s">
         <v>0</v>
@@ -3384,8 +3782,14 @@
       <c r="G87" s="33" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="H87" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="I87" s="33" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88" s="6">
         <v>1</v>
       </c>
@@ -3399,14 +3803,18 @@
         <v>226</v>
       </c>
       <c r="E88" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F88" s="26"/>
       <c r="G88" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="H88" s="26"/>
+      <c r="I88" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89" s="3">
         <v>2</v>
       </c>
@@ -3426,8 +3834,12 @@
         <v>315</v>
       </c>
       <c r="G89" s="25"/>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="H89" s="26"/>
+      <c r="I89" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90" s="6">
         <v>3</v>
       </c>
@@ -3447,8 +3859,12 @@
       <c r="G90" s="27">
         <v>80</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90" s="26"/>
+      <c r="I90" s="27">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" s="3">
         <v>4</v>
       </c>
@@ -3468,8 +3884,12 @@
         <v>319</v>
       </c>
       <c r="G91" s="25"/>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="H91" s="26" t="s">
+        <v>322</v>
+      </c>
+      <c r="I91" s="25"/>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92" s="6">
         <v>5</v>
       </c>
@@ -3483,14 +3903,18 @@
         <v>13</v>
       </c>
       <c r="E92" s="22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F92" s="26"/>
       <c r="G92" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="H92" s="26"/>
+      <c r="I92" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" s="3">
         <v>6</v>
       </c>
@@ -3510,8 +3934,12 @@
         <v>315</v>
       </c>
       <c r="G93" s="25"/>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="H93" s="26"/>
+      <c r="I93" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94" s="6">
         <v>7</v>
       </c>
@@ -3531,8 +3959,12 @@
       <c r="G94" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="H94" s="26"/>
+      <c r="I94" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95" s="3">
         <v>8</v>
       </c>
@@ -3552,8 +3984,12 @@
         <v>315</v>
       </c>
       <c r="G95" s="25"/>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="H95" s="26"/>
+      <c r="I95" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96" s="6">
         <v>9</v>
       </c>
@@ -3573,8 +4009,12 @@
       <c r="G96" s="27">
         <v>80</v>
       </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="H96" s="26"/>
+      <c r="I96" s="27">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97" s="3">
         <v>10</v>
       </c>
@@ -3594,8 +4034,12 @@
         <v>315</v>
       </c>
       <c r="G97" s="25"/>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="H97" s="26"/>
+      <c r="I97" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98" s="6">
         <v>11</v>
       </c>
@@ -3615,8 +4059,12 @@
         <v>315</v>
       </c>
       <c r="G98" s="25"/>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="H98" s="26"/>
+      <c r="I98" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99" s="3">
         <v>12</v>
       </c>
@@ -3636,8 +4084,12 @@
       <c r="G99" s="27">
         <v>50</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="H99" s="26"/>
+      <c r="I99" s="27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100" s="6">
         <v>13</v>
       </c>
@@ -3657,8 +4109,12 @@
         <v>315</v>
       </c>
       <c r="G100" s="25"/>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="H100" s="26"/>
+      <c r="I100" s="25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101" s="3">
         <v>14</v>
       </c>
@@ -3678,8 +4134,12 @@
         <v>315</v>
       </c>
       <c r="G101" s="25"/>
-    </row>
-    <row r="102" spans="1:7">
+      <c r="H101" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I101" s="25"/>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102" s="6">
         <v>15</v>
       </c>
@@ -3699,8 +4159,12 @@
         <v>315</v>
       </c>
       <c r="G102" s="25"/>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="H102" s="26"/>
+      <c r="I102" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103" s="3">
         <v>16</v>
       </c>
@@ -3720,8 +4184,12 @@
         <v>315</v>
       </c>
       <c r="G103" s="25"/>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="H103" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I103" s="25"/>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104" s="6">
         <v>17</v>
       </c>
@@ -3741,8 +4209,12 @@
         <v>315</v>
       </c>
       <c r="G104" s="25"/>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="H104" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I104" s="25"/>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105" s="3">
         <v>18</v>
       </c>
@@ -3762,8 +4234,12 @@
       <c r="G105" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="H105" s="26"/>
+      <c r="I105" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
       <c r="A106" s="6">
         <v>19</v>
       </c>
@@ -3783,8 +4259,12 @@
       <c r="G106" s="27">
         <v>90</v>
       </c>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="H106" s="26"/>
+      <c r="I106" s="27">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
       <c r="A107" s="3">
         <v>20</v>
       </c>
@@ -3804,8 +4284,12 @@
         <v>315</v>
       </c>
       <c r="G107" s="25"/>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="H107" s="26"/>
+      <c r="I107" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
       <c r="A108" s="6">
         <v>21</v>
       </c>
@@ -3825,8 +4309,12 @@
         <v>315</v>
       </c>
       <c r="G108" s="25"/>
-    </row>
-    <row r="109" spans="1:7">
+      <c r="H108" s="26" t="s">
+        <v>315</v>
+      </c>
+      <c r="I108" s="25"/>
+    </row>
+    <row r="109" spans="1:9">
       <c r="A109" s="3">
         <v>22</v>
       </c>
@@ -3846,8 +4334,12 @@
         <v>315</v>
       </c>
       <c r="G109" s="25"/>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="H109" s="26"/>
+      <c r="I109" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
       <c r="A110" s="6">
         <v>23</v>
       </c>
@@ -3867,8 +4359,10 @@
         <v>315</v>
       </c>
       <c r="G110" s="25"/>
-    </row>
-    <row r="111" spans="1:7">
+      <c r="H110" s="26"/>
+      <c r="I110" s="25"/>
+    </row>
+    <row r="111" spans="1:9">
       <c r="A111" s="3">
         <v>24</v>
       </c>
@@ -3885,9 +4379,15 @@
         <v>3</v>
       </c>
       <c r="F111" s="24"/>
-      <c r="G111" s="27"/>
-    </row>
-    <row r="112" spans="1:7">
+      <c r="G111" s="27">
+        <v>50</v>
+      </c>
+      <c r="H111" s="26"/>
+      <c r="I111" s="27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
       <c r="A112" s="6">
         <v>25</v>
       </c>
@@ -3907,8 +4407,12 @@
       <c r="G112" s="27">
         <v>85</v>
       </c>
-    </row>
-    <row r="113" spans="1:7">
+      <c r="H112" s="26"/>
+      <c r="I112" s="27">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
       <c r="A113" s="3">
         <v>26</v>
       </c>
@@ -3926,8 +4430,12 @@
       </c>
       <c r="F113" s="24"/>
       <c r="G113" s="27"/>
-    </row>
-    <row r="114" spans="1:7">
+      <c r="H113" s="26"/>
+      <c r="I113" s="27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
       <c r="A114" s="6">
         <v>27</v>
       </c>
@@ -3947,8 +4455,12 @@
       <c r="G114" s="27">
         <v>85</v>
       </c>
-    </row>
-    <row r="115" spans="1:7">
+      <c r="H114" s="26"/>
+      <c r="I114" s="27">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
       <c r="A115" s="3">
         <v>28</v>
       </c>
@@ -3968,8 +4480,12 @@
         <v>315</v>
       </c>
       <c r="G115" s="25"/>
-    </row>
-    <row r="116" spans="1:7">
+      <c r="H115" s="26"/>
+      <c r="I115" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
       <c r="A116" s="6">
         <v>29</v>
       </c>
@@ -3988,11 +4504,13 @@
       <c r="F116" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="G116" s="27">
+      <c r="G116" s="27"/>
+      <c r="H116" s="26"/>
+      <c r="I116" s="27">
         <v>70</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:9">
       <c r="A117" s="3">
         <v>30</v>
       </c>
@@ -4012,8 +4530,12 @@
       <c r="G117" s="25">
         <v>50</v>
       </c>
-    </row>
-    <row r="118" spans="1:7">
+      <c r="H117" s="26"/>
+      <c r="I117" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
       <c r="A118" s="6">
         <v>31</v>
       </c>
@@ -4033,8 +4555,12 @@
       <c r="G118" s="27">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:7">
+      <c r="H118" s="26"/>
+      <c r="I118" s="27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
       <c r="A119" s="3">
         <v>32</v>
       </c>
@@ -4054,8 +4580,12 @@
       <c r="G119" s="27">
         <v>70</v>
       </c>
-    </row>
-    <row r="120" spans="1:7">
+      <c r="H119" s="26"/>
+      <c r="I119" s="27">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
       <c r="A120" s="6">
         <v>33</v>
       </c>
@@ -4075,8 +4605,12 @@
         <v>315</v>
       </c>
       <c r="G120" s="25"/>
-    </row>
-    <row r="121" spans="1:7">
+      <c r="H120" s="26"/>
+      <c r="I120" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
       <c r="A121" s="3">
         <v>34</v>
       </c>
@@ -4096,8 +4630,12 @@
         <v>315</v>
       </c>
       <c r="G121" s="25"/>
-    </row>
-    <row r="122" spans="1:7">
+      <c r="H121" s="26"/>
+      <c r="I121" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
       <c r="A122" s="6">
         <v>35</v>
       </c>
@@ -4117,8 +4655,12 @@
         <v>315</v>
       </c>
       <c r="G122" s="25"/>
-    </row>
-    <row r="123" spans="1:7">
+      <c r="H122" s="26"/>
+      <c r="I122" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
       <c r="A123" s="3">
         <v>36</v>
       </c>
@@ -4138,8 +4680,12 @@
         <v>315</v>
       </c>
       <c r="G123" s="25"/>
-    </row>
-    <row r="124" spans="1:7">
+      <c r="H123" s="26"/>
+      <c r="I123" s="25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
       <c r="A124" s="6">
         <v>37</v>
       </c>
@@ -4159,14 +4705,24 @@
         <v>315</v>
       </c>
       <c r="G124" s="25"/>
-    </row>
-    <row r="140" spans="7:7">
+      <c r="H124" s="26"/>
+      <c r="I124" s="25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="140" spans="7:9">
       <c r="G140" s="20" t="s">
         <v>316</v>
       </c>
+      <c r="I140" s="20" t="s">
+        <v>316</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="10">
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H86:I86"/>
     <mergeCell ref="F86:G86"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A2:C2"/>

</xml_diff>